<commit_message>
Added command table for assignment 9
</commit_message>
<xml_diff>
--- a/questions/Assignment 8 - Blue Gecko Command Table.xlsx
+++ b/questions/Assignment 8 - Blue Gecko Command Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohit\SimplicityStudio\v4_workspace\ecen5823-assignments\questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0A3923-AC40-4324-AC15-612B79F74F91}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747CEC96-6CE0-4A09-A094-31688587EAD8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="145">
   <si>
     <t>Event Handler Event</t>
   </si>
@@ -373,15 +373,6 @@
     <t>Gets the latest rssi</t>
   </si>
   <si>
-    <t>Assignment 8</t>
-  </si>
-  <si>
-    <t>evt_sm_confirm_bonding</t>
-  </si>
-  <si>
-    <t>https://docs.silabs.com/bluetooth/latest/sm#evt_sm_confirm_bonding</t>
-  </si>
-  <si>
     <t>https://docs.silabs.com/bluetooth/latest/sm#evt_sm_confirm_passkey</t>
   </si>
   <si>
@@ -397,21 +388,6 @@
     <t>evt_sm_bonding_failed</t>
   </si>
   <si>
-    <t>https://docs.silabs.com/bluetooth/latest/sm#cmd_sm_bonding_confirm</t>
-  </si>
-  <si>
-    <t>cmd_sm_bonding_confirm</t>
-  </si>
-  <si>
-    <t>cmd_sm_passkey_confirm</t>
-  </si>
-  <si>
-    <t>https://docs.silabs.com/bluetooth/latest/sm#cmd_sm_passkey_confirm</t>
-  </si>
-  <si>
-    <t>connection, confirm</t>
-  </si>
-  <si>
     <t>"Bonded"</t>
   </si>
   <si>
@@ -424,29 +400,68 @@
     <t>cmd_sm_increase_security</t>
   </si>
   <si>
-    <t>at gpio interrupt</t>
-  </si>
-  <si>
     <t>https://docs.silabs.com/bluetooth/latest/sm#cmd_sm_increase_security</t>
   </si>
   <si>
     <t>connection</t>
   </si>
   <si>
-    <t>cmd_sm_delete_bondings, cmd_sm_configure</t>
-  </si>
-  <si>
     <t>https://docs.silabs.com/bluetooth/latest/sm#cmd_sm_delete_bondings https://docs.silabs.com/bluetooth/latest/sm#cmd_sm_configure</t>
   </si>
   <si>
-    <t>flgas, io_capabilities</t>
+    <t>cmd_sm_delete_bondings, cmd_sm_configure, cmd_sm_set_bondable_mode</t>
+  </si>
+  <si>
+    <t>cmd_sm_delete_bondings</t>
+  </si>
+  <si>
+    <t>https://docs.silabs.com/bluetooth/latest/sm#cmd_sm_delete_bondings</t>
+  </si>
+  <si>
+    <t>Sending cmd_sm_passkey_confirm from external event</t>
+  </si>
+  <si>
+    <t>see above</t>
+  </si>
+  <si>
+    <t>Deleting all bondings and configuring security settings</t>
+  </si>
+  <si>
+    <t>Deleting all bondings</t>
+  </si>
+  <si>
+    <t>Displaying "Bonded" when bonding is done successfully</t>
+  </si>
+  <si>
+    <t>Displaying "Bonding Failed" when bonding is not done</t>
+  </si>
+  <si>
+    <t>flags, io_capabilities; sm_configure - 0x01, sm_io_capability_displayyesno</t>
+  </si>
+  <si>
+    <t>gecko_evt_gatt_characteristic_value</t>
+  </si>
+  <si>
+    <t>"Button State: X"</t>
+  </si>
+  <si>
+    <t>Assignment 9 - additional</t>
+  </si>
+  <si>
+    <t>Assignment 8 - additional</t>
+  </si>
+  <si>
+    <t>Sending cmd_sm_passkey_confirmation to server</t>
+  </si>
+  <si>
+    <t>same as above for this state</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -545,6 +560,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -586,7 +606,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -631,6 +651,9 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -949,19 +972,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AJ979"/>
+  <dimension ref="A1:AJ976"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="31.44140625" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.88671875" customWidth="1"/>
-    <col min="4" max="4" width="41.88671875" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" customWidth="1"/>
+    <col min="4" max="4" width="31" customWidth="1"/>
     <col min="5" max="5" width="21.5546875" customWidth="1"/>
     <col min="8" max="8" width="19.33203125" customWidth="1"/>
     <col min="9" max="9" width="21.33203125" customWidth="1"/>
@@ -1613,7 +1636,7 @@
       <c r="A13" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="19" t="s">
         <v>72</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -2063,45 +2086,78 @@
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1">
       <c r="A27" s="20" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1">
       <c r="A28" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="19" t="s">
         <v>15</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="E28" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="F28" s="21" t="s">
         <v>138</v>
-      </c>
-      <c r="F28" s="21" t="s">
-        <v>139</v>
       </c>
       <c r="G28" s="22"/>
       <c r="H28" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="I28" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M28" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N28" s="5" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1">
       <c r="A29" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C29" t="s">
         <v>16</v>
       </c>
+      <c r="D29" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" t="s">
+        <v>18</v>
+      </c>
       <c r="H29" s="22" t="s">
-        <v>131</v>
+        <v>123</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="J29" s="5" t="s">
         <v>18</v>
@@ -2109,140 +2165,439 @@
       <c r="K29" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="L29" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M29" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N29" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A30" s="22" t="s">
-        <v>134</v>
+      <c r="A30" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>42</v>
       </c>
       <c r="C30" t="s">
         <v>16</v>
       </c>
       <c r="D30" t="s">
-        <v>127</v>
-      </c>
-      <c r="E30" s="19" t="s">
-        <v>128</v>
+        <v>18</v>
+      </c>
+      <c r="E30" t="s">
+        <v>18</v>
       </c>
       <c r="F30" t="s">
-        <v>129</v>
+        <v>18</v>
+      </c>
+      <c r="G30" t="s">
+        <v>18</v>
+      </c>
+      <c r="H30" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J30" t="s">
+        <v>18</v>
+      </c>
+      <c r="K30" t="s">
+        <v>18</v>
+      </c>
+      <c r="L30" t="s">
+        <v>18</v>
+      </c>
+      <c r="M30" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N30" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="15.75" customHeight="1">
       <c r="A31" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>33</v>
+        <v>121</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>120</v>
       </c>
       <c r="C31" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="E31" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="F31" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="J31" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="K31" s="3" t="s">
+      <c r="D31" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" t="s">
+        <v>18</v>
+      </c>
+      <c r="H31" s="22" t="s">
         <v>124</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J31" t="s">
+        <v>18</v>
+      </c>
+      <c r="K31" t="s">
+        <v>18</v>
+      </c>
+      <c r="L31" t="s">
+        <v>18</v>
+      </c>
+      <c r="M31" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N31" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1">
       <c r="A32" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" t="s">
+        <v>130</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="F32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" t="s">
+        <v>18</v>
+      </c>
+      <c r="H32" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M32" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N32" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="13.2">
+      <c r="A34" s="12"/>
+    </row>
+    <row r="35" spans="1:14" ht="13.2">
+      <c r="A35" s="20" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="13.2">
+      <c r="A36" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" t="s">
+        <v>130</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="F36" t="s">
+        <v>18</v>
+      </c>
+      <c r="G36" t="s">
+        <v>18</v>
+      </c>
+      <c r="H36" t="s">
+        <v>133</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L36" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M36" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N36" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="13.2">
+      <c r="A37" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" t="s">
+        <v>130</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="F37" t="s">
+        <v>18</v>
+      </c>
+      <c r="G37" t="s">
+        <v>18</v>
+      </c>
+      <c r="H37" t="s">
+        <v>133</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L37" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M37" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N37" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="13.2">
+      <c r="A38" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" t="s">
+        <v>125</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="F38" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="G38" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="H38" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="L38" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M38" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N38" s="22" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="13.2">
+      <c r="A39" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" t="s">
+        <v>18</v>
+      </c>
+      <c r="E39" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" t="s">
+        <v>18</v>
+      </c>
+      <c r="G39" t="s">
+        <v>18</v>
+      </c>
+      <c r="H39" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="B32" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" t="s">
-        <v>16</v>
-      </c>
-      <c r="H32" s="22" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A33" s="3" t="s">
+      <c r="I39" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L39" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M39" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N39" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="13.2">
+      <c r="A40" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" t="s">
+        <v>18</v>
+      </c>
+      <c r="G40" t="s">
+        <v>18</v>
+      </c>
+      <c r="H40" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="B33" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="C33" t="s">
-        <v>16</v>
-      </c>
-      <c r="H33" s="22" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="13.2">
-      <c r="A36" s="12"/>
-    </row>
-    <row r="37" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A37" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B37" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="C37" t="s">
-        <v>16</v>
-      </c>
-      <c r="D37" t="s">
-        <v>126</v>
-      </c>
-      <c r="E37" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="F37" t="s">
-        <v>129</v>
-      </c>
-      <c r="J37" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K37" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="13.2">
-      <c r="A38" s="12"/>
-    </row>
-    <row r="39" spans="1:11" ht="13.2">
-      <c r="A39" s="12"/>
-    </row>
-    <row r="40" spans="1:11" ht="13.2">
-      <c r="A40" s="12"/>
-    </row>
-    <row r="41" spans="1:11" ht="13.2">
-      <c r="A41" s="12"/>
-      <c r="C41" s="22"/>
-      <c r="E41" s="19"/>
-    </row>
-    <row r="42" spans="1:11" ht="13.2">
+      <c r="I40" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K40" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L40" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M40" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N40" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="13.2">
+      <c r="A41" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="E41" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="F41" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="G41" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="H41" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J41" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="K41" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="L41" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="M41" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="N41" s="22" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="13.2">
       <c r="A42" s="12"/>
     </row>
-    <row r="43" spans="1:11" ht="13.2">
+    <row r="43" spans="1:14" ht="13.2">
       <c r="A43" s="12"/>
     </row>
-    <row r="44" spans="1:11" ht="13.2">
+    <row r="44" spans="1:14" ht="13.2">
       <c r="A44" s="12"/>
     </row>
-    <row r="45" spans="1:11" ht="13.2">
+    <row r="45" spans="1:14" ht="13.2">
       <c r="A45" s="12"/>
     </row>
-    <row r="46" spans="1:11" ht="13.2">
+    <row r="46" spans="1:14" ht="13.2">
       <c r="A46" s="12"/>
     </row>
-    <row r="47" spans="1:11" ht="13.2">
+    <row r="47" spans="1:14" ht="13.2">
       <c r="A47" s="12"/>
     </row>
-    <row r="48" spans="1:11" ht="13.2">
+    <row r="48" spans="1:14" ht="13.2">
       <c r="A48" s="12"/>
     </row>
     <row r="49" spans="1:1" ht="13.2">
@@ -5028,15 +5383,6 @@
     </row>
     <row r="976" spans="1:1" ht="13.2">
       <c r="A976" s="12"/>
-    </row>
-    <row r="977" spans="1:1" ht="13.2">
-      <c r="A977" s="12"/>
-    </row>
-    <row r="978" spans="1:1" ht="13.2">
-      <c r="A978" s="12"/>
-    </row>
-    <row r="979" spans="1:1" ht="13.2">
-      <c r="A979" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5066,19 +5412,24 @@
     <hyperlink ref="B16" r:id="rId24" location="evt_system_external_signal" xr:uid="{6BA9AC43-BDEA-414D-AD75-82C1BDD7F3DD}"/>
     <hyperlink ref="E11" r:id="rId25" location="cmd_gatt_set_characteristic_notification" xr:uid="{E11EC0C2-1802-4031-B3BC-6B9D0B030616}"/>
     <hyperlink ref="B29" r:id="rId26" location="evt_sm_confirm_passkey" xr:uid="{14E85C68-6D3C-440C-AE3B-AAD57C82CA3E}"/>
-    <hyperlink ref="B32" r:id="rId27" location="evt_sm_bonded" xr:uid="{A0F7B211-5393-4671-BC7A-523EC2F65E13}"/>
-    <hyperlink ref="B33" r:id="rId28" location="evt_sm_bonding_failed" xr:uid="{0BE6D36D-FDBF-442F-A52C-6810E2700686}"/>
+    <hyperlink ref="B30" r:id="rId27" location="evt_sm_bonded" xr:uid="{A0F7B211-5393-4671-BC7A-523EC2F65E13}"/>
+    <hyperlink ref="B31" r:id="rId28" location="evt_sm_bonding_failed" xr:uid="{0BE6D36D-FDBF-442F-A52C-6810E2700686}"/>
     <hyperlink ref="B17" r:id="rId29" location="evt_le_connection_rssi" xr:uid="{0C36A87E-B372-4733-BE4C-0A0F758742DF}"/>
     <hyperlink ref="B18" r:id="rId30" location="evt_gatt_server_characteristic_status" xr:uid="{4CD74F28-5169-4A95-9F7D-35D5050BE574}"/>
     <hyperlink ref="E28" r:id="rId31" location="cmd_sm_delete_bondings, " display="https://docs.silabs.com/bluetooth/latest/sm#cmd_sm_delete_bondings, " xr:uid="{BB33249D-42B1-46DB-A7C4-2A43E48A1378}"/>
     <hyperlink ref="B28" r:id="rId32" location="evt_system_boot" xr:uid="{66ACADCD-3286-477A-ABB6-57512EE79561}"/>
-    <hyperlink ref="E37" r:id="rId33" location="cmd_sm_bonding_confirm" xr:uid="{6C7EB2EE-F568-45D2-8ACF-CF23A3747315}"/>
-    <hyperlink ref="B37" r:id="rId34" location="evt_sm_confirm_bonding" xr:uid="{805E772B-D950-4115-A5B6-D2E35F1CC03A}"/>
-    <hyperlink ref="B31" r:id="rId35" location="evt_le_connection_opened" xr:uid="{00C76DC6-BCF3-4EEB-9CB4-E719FF8B9A2F}"/>
-    <hyperlink ref="E31" r:id="rId36" location="cmd_sm_increase_security" xr:uid="{6B227684-9A23-4CEC-BD45-7AE9BF5CFC24}"/>
-    <hyperlink ref="E30" r:id="rId37" location="cmd_sm_passkey_confirm" xr:uid="{A39625F7-B36C-4D03-8707-E4523EC83C10}"/>
+    <hyperlink ref="B32" r:id="rId33" location="evt_le_connection_closed" xr:uid="{FB973842-DC54-4C76-84D5-3409E68323AB}"/>
+    <hyperlink ref="E32" r:id="rId34" location="cmd_sm_delete_bondings" xr:uid="{A96C6D10-B410-4765-A2A6-C6564A3DDCB3}"/>
+    <hyperlink ref="E36" r:id="rId35" location="cmd_sm_delete_bondings" xr:uid="{A01D8C18-6439-45BE-81B7-65158E72E312}"/>
+    <hyperlink ref="E37" r:id="rId36" location="cmd_sm_delete_bondings" xr:uid="{8B744716-267D-47D0-97D6-2EE5FCB08993}"/>
+    <hyperlink ref="B38" r:id="rId37" location="evt_sm_confirm_passkey" xr:uid="{5F8A14A8-0FD8-4BEC-AA20-0FB0AFE6E548}"/>
+    <hyperlink ref="B39" r:id="rId38" location="evt_sm_bonded" xr:uid="{A82A361A-E810-4617-A1A7-7114B1A0B58E}"/>
+    <hyperlink ref="B40" r:id="rId39" location="evt_sm_bonding_failed" xr:uid="{FD30E1A7-EF75-4420-ADE2-4EF277C9E698}"/>
+    <hyperlink ref="B37" r:id="rId40" location="evt_le_connection_closed" xr:uid="{04A92649-A104-4A56-B2F8-826286EE6A7A}"/>
+    <hyperlink ref="B36" r:id="rId41" location="evt_system_boot" xr:uid="{8312EAFF-6A90-4703-87FD-4A9FB12B4644}"/>
+    <hyperlink ref="B41" r:id="rId42" location="evt_gatt_characteristic_value" xr:uid="{A843C51F-02F1-40CB-ABA5-5B08C15B7C97}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId38"/>
+  <pageSetup orientation="portrait" r:id="rId43"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Assignment 8 updated with flash erase command
</commit_message>
<xml_diff>
--- a/questions/Assignment 8 - Blue Gecko Command Table.xlsx
+++ b/questions/Assignment 8 - Blue Gecko Command Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohit\SimplicityStudio\v4_workspace\ecen5823-assignments\questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C29628-6598-4E86-AE76-629B1E647C8A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC739AC0-7BE1-4DB2-8D16-48DD2B2F5AA3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="16395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment 67 Without Bonding" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="146">
   <si>
     <t>Event Handler Event</t>
   </si>
@@ -409,9 +409,6 @@
     <t>https://docs.silabs.com/bluetooth/latest/sm#cmd_sm_delete_bondings https://docs.silabs.com/bluetooth/latest/sm#cmd_sm_configure</t>
   </si>
   <si>
-    <t>cmd_sm_delete_bondings, cmd_sm_configure, cmd_sm_set_bondable_mode</t>
-  </si>
-  <si>
     <t>cmd_sm_delete_bondings</t>
   </si>
   <si>
@@ -455,6 +452,12 @@
   </si>
   <si>
     <t>same as above for this state</t>
+  </si>
+  <si>
+    <t>cmd_sm_delete_bondings, cmd_flash_ps_erase_all</t>
+  </si>
+  <si>
+    <t>cmd_sm_delete_bondings, cmd_sm_configure, cmd_sm_set_bondable_mode, cmd_flash_ps_erase_all</t>
   </si>
 </sst>
 </file>
@@ -975,8 +978,8 @@
   <dimension ref="A1:AJ976"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2086,7 +2089,7 @@
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1">
       <c r="A27" s="20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1">
@@ -2100,13 +2103,13 @@
         <v>16</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
       <c r="E28" s="23" t="s">
         <v>128</v>
       </c>
       <c r="F28" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G28" s="22"/>
       <c r="H28" s="5" t="s">
@@ -2128,7 +2131,7 @@
         <v>18</v>
       </c>
       <c r="N28" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1">
@@ -2172,7 +2175,7 @@
         <v>18</v>
       </c>
       <c r="N29" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1">
@@ -2216,7 +2219,7 @@
         <v>18</v>
       </c>
       <c r="N30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="15.75" customHeight="1">
@@ -2260,7 +2263,7 @@
         <v>18</v>
       </c>
       <c r="N31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1">
@@ -2274,10 +2277,10 @@
         <v>16</v>
       </c>
       <c r="D32" t="s">
+        <v>144</v>
+      </c>
+      <c r="E32" s="19" t="s">
         <v>130</v>
-      </c>
-      <c r="E32" s="19" t="s">
-        <v>131</v>
       </c>
       <c r="F32" t="s">
         <v>18</v>
@@ -2304,7 +2307,7 @@
         <v>18</v>
       </c>
       <c r="N32" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="13.2">
@@ -2312,7 +2315,7 @@
     </row>
     <row r="35" spans="1:14" ht="13.2">
       <c r="A35" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="13.2">
@@ -2326,11 +2329,11 @@
         <v>19</v>
       </c>
       <c r="D36" t="s">
+        <v>129</v>
+      </c>
+      <c r="E36" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="E36" s="19" t="s">
-        <v>131</v>
-      </c>
       <c r="F36" t="s">
         <v>18</v>
       </c>
@@ -2338,7 +2341,7 @@
         <v>18</v>
       </c>
       <c r="H36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I36" s="5" t="s">
         <v>18</v>
@@ -2356,7 +2359,7 @@
         <v>18</v>
       </c>
       <c r="N36" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="13.2">
@@ -2370,11 +2373,11 @@
         <v>19</v>
       </c>
       <c r="D37" t="s">
+        <v>129</v>
+      </c>
+      <c r="E37" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="E37" s="19" t="s">
-        <v>131</v>
-      </c>
       <c r="F37" t="s">
         <v>18</v>
       </c>
@@ -2382,7 +2385,7 @@
         <v>18</v>
       </c>
       <c r="H37" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I37" s="5" t="s">
         <v>18</v>
@@ -2400,7 +2403,7 @@
         <v>18</v>
       </c>
       <c r="N37" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="13.2">
@@ -2444,7 +2447,7 @@
         <v>18</v>
       </c>
       <c r="N38" s="22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="13.2">
@@ -2488,7 +2491,7 @@
         <v>18</v>
       </c>
       <c r="N39" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="13.2">
@@ -2532,12 +2535,12 @@
         <v>18</v>
       </c>
       <c r="N40" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="13.2">
       <c r="A41" s="24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B41" s="19" t="s">
         <v>72</v>
@@ -2546,37 +2549,37 @@
         <v>19</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F41" s="22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G41" s="22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H41" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I41" s="5" t="s">
         <v>18</v>
       </c>
       <c r="J41" s="22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K41" s="22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L41" s="22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="M41" s="22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N41" s="22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="13.2">

</xml_diff>